<commit_message>
Notification module excel file data entry issues fixed
</commit_message>
<xml_diff>
--- a/public/seeders/email_notifications.xlsx
+++ b/public/seeders/email_notifications.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farosh3\Videos\AnyDesk\saas-boilerplate\storage\app\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farosh3\Videos\AnyDesk\saas-boilerplate\public\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="331">
   <si>
     <t>Notification</t>
   </si>
@@ -1950,12 +1950,15 @@
   <si>
     <t>Staff</t>
   </si>
+  <si>
+    <t>Type of Trigger</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2005,6 +2008,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2053,7 +2064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2145,6 +2156,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2533,6 +2547,116 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="image3.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9591675" y="103260525"/>
+          <a:ext cx="180975" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9591675" y="103260525"/>
+          <a:ext cx="180975" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2733,15 +2857,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AC1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L2" sqref="L2:L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2750,9 +2874,10 @@
     <col min="2" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="5" width="26.7109375" customWidth="1"/>
     <col min="6" max="11" width="34.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2786,7 +2911,9 @@
       <c r="K1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="6"/>
+      <c r="L1" s="32" t="s">
+        <v>330</v>
+      </c>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -2839,7 +2966,9 @@
       <c r="K2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="9">
+        <v>2</v>
+      </c>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
@@ -2892,7 +3021,9 @@
       <c r="K3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="9">
+        <v>2</v>
+      </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -2945,7 +3076,9 @@
       <c r="K4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="9">
+        <v>2</v>
+      </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -2998,7 +3131,9 @@
       <c r="K5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="9">
+        <v>2</v>
+      </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -3051,7 +3186,9 @@
       <c r="K6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="9">
+        <v>2</v>
+      </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -3104,7 +3241,9 @@
       <c r="K7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="9">
+        <v>2</v>
+      </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -3157,7 +3296,9 @@
       <c r="K8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="9">
+        <v>2</v>
+      </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -3210,7 +3351,9 @@
       <c r="K9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="9">
+        <v>2</v>
+      </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -3229,7 +3372,7 @@
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
     </row>
-    <row r="10" spans="1:29" ht="395.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>45</v>
       </c>
@@ -3263,7 +3406,9 @@
       <c r="K10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="9">
+        <v>2</v>
+      </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -3316,7 +3461,9 @@
       <c r="K11" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="9">
+        <v>2</v>
+      </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -3369,7 +3516,9 @@
       <c r="K12" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="9">
+        <v>2</v>
+      </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -3388,7 +3537,7 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="357" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="369.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>59</v>
       </c>
@@ -3422,7 +3571,9 @@
       <c r="K13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="9">
+        <v>2</v>
+      </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -3441,7 +3592,7 @@
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
     </row>
-    <row r="14" spans="1:29" ht="344.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="357" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>64</v>
       </c>
@@ -3475,7 +3626,9 @@
       <c r="K14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L14" s="14"/>
+      <c r="L14" s="9">
+        <v>2</v>
+      </c>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
@@ -3528,7 +3681,9 @@
       <c r="K15" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="L15" s="6"/>
+      <c r="L15" s="9">
+        <v>2</v>
+      </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
@@ -3581,7 +3736,9 @@
       <c r="K16" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="L16" s="6"/>
+      <c r="L16" s="9">
+        <v>2</v>
+      </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -3634,7 +3791,9 @@
       <c r="K17" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="6"/>
+      <c r="L17" s="9">
+        <v>2</v>
+      </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
@@ -3687,7 +3846,9 @@
       <c r="K18" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="L18" s="6"/>
+      <c r="L18" s="9">
+        <v>2</v>
+      </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -3706,7 +3867,7 @@
       <c r="AB18" s="6"/>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="357" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="369.75" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>90</v>
       </c>
@@ -3740,7 +3901,9 @@
       <c r="K19" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="L19" s="6"/>
+      <c r="L19" s="9">
+        <v>2</v>
+      </c>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -3793,7 +3956,9 @@
       <c r="K20" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="L20" s="9">
+        <v>2</v>
+      </c>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -3846,7 +4011,9 @@
       <c r="K21" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="9">
+        <v>2</v>
+      </c>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -3899,7 +4066,9 @@
       <c r="K22" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="L22" s="6"/>
+      <c r="L22" s="9">
+        <v>2</v>
+      </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -3952,7 +4121,9 @@
       <c r="K23" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="L23" s="6"/>
+      <c r="L23" s="9">
+        <v>2</v>
+      </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -4005,7 +4176,9 @@
       <c r="K24" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="L24" s="6"/>
+      <c r="L24" s="9">
+        <v>2</v>
+      </c>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
@@ -4024,7 +4197,7 @@
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
     </row>
-    <row r="25" spans="1:29" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="153" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>123</v>
       </c>
@@ -4058,7 +4231,9 @@
       <c r="K25" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="L25" s="6"/>
+      <c r="L25" s="9">
+        <v>2</v>
+      </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
@@ -4095,7 +4270,9 @@
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
-      <c r="L26" s="6"/>
+      <c r="L26" s="9">
+        <v>2</v>
+      </c>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
@@ -4148,7 +4325,9 @@
       <c r="K27" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="L27" s="6"/>
+      <c r="L27" s="9">
+        <v>2</v>
+      </c>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
@@ -4167,7 +4346,7 @@
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
     </row>
-    <row r="28" spans="1:29" ht="255" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="267.75" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>134</v>
       </c>
@@ -4201,7 +4380,9 @@
       <c r="K28" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="L28" s="6"/>
+      <c r="L28" s="9">
+        <v>2</v>
+      </c>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -4244,7 +4425,9 @@
       <c r="K29" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="L29" s="6"/>
+      <c r="L29" s="9">
+        <v>2</v>
+      </c>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -4263,7 +4446,7 @@
       <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
     </row>
-    <row r="30" spans="1:29" ht="216.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>141</v>
       </c>
@@ -4297,7 +4480,9 @@
       <c r="K30" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="L30" s="6"/>
+      <c r="L30" s="9">
+        <v>2</v>
+      </c>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -4350,7 +4535,9 @@
       <c r="K31" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="L31" s="6"/>
+      <c r="L31" s="9">
+        <v>2</v>
+      </c>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
@@ -4403,7 +4590,9 @@
       <c r="K32" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="L32" s="6"/>
+      <c r="L32" s="9">
+        <v>2</v>
+      </c>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
@@ -4422,7 +4611,7 @@
       <c r="AB32" s="6"/>
       <c r="AC32" s="6"/>
     </row>
-    <row r="33" spans="1:29" ht="293.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" ht="306" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>158</v>
       </c>
@@ -4456,7 +4645,9 @@
       <c r="K33" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="L33" s="6"/>
+      <c r="L33" s="9">
+        <v>2</v>
+      </c>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
@@ -4475,7 +4666,7 @@
       <c r="AB33" s="6"/>
       <c r="AC33" s="6"/>
     </row>
-    <row r="34" spans="1:29" ht="318.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" ht="331.5" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>165</v>
       </c>
@@ -4509,7 +4700,9 @@
       <c r="K34" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="L34" s="6"/>
+      <c r="L34" s="9">
+        <v>2</v>
+      </c>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
@@ -4528,7 +4721,7 @@
       <c r="AB34" s="6"/>
       <c r="AC34" s="6"/>
     </row>
-    <row r="35" spans="1:29" ht="267.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" ht="280.5" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>169</v>
       </c>
@@ -4562,7 +4755,9 @@
       <c r="K35" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="L35" s="6"/>
+      <c r="L35" s="9">
+        <v>2</v>
+      </c>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
@@ -4615,7 +4810,9 @@
       <c r="K36" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="L36" s="6"/>
+      <c r="L36" s="9">
+        <v>2</v>
+      </c>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
@@ -4668,7 +4865,9 @@
       <c r="K37" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="L37" s="6"/>
+      <c r="L37" s="9">
+        <v>2</v>
+      </c>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
@@ -4721,7 +4920,9 @@
       <c r="K38" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L38" s="26"/>
+      <c r="L38" s="9">
+        <v>2</v>
+      </c>
       <c r="M38" s="26"/>
       <c r="N38" s="26"/>
       <c r="O38" s="26"/>
@@ -4740,7 +4941,7 @@
       <c r="AB38" s="26"/>
       <c r="AC38" s="26"/>
     </row>
-    <row r="39" spans="1:29" ht="293.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" ht="306" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>189</v>
       </c>
@@ -4774,7 +4975,9 @@
       <c r="K39" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="L39" s="26"/>
+      <c r="L39" s="9">
+        <v>2</v>
+      </c>
       <c r="M39" s="26"/>
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
@@ -4827,7 +5030,9 @@
       <c r="K40" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L40" s="6"/>
+      <c r="L40" s="9">
+        <v>2</v>
+      </c>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
@@ -4846,7 +5051,7 @@
       <c r="AB40" s="6"/>
       <c r="AC40" s="6"/>
     </row>
-    <row r="41" spans="1:29" ht="331.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" ht="344.25" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>196</v>
       </c>
@@ -4880,7 +5085,9 @@
       <c r="K41" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="L41" s="6"/>
+      <c r="L41" s="9">
+        <v>2</v>
+      </c>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
@@ -4933,7 +5140,9 @@
       <c r="K42" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="L42" s="6"/>
+      <c r="L42" s="9">
+        <v>2</v>
+      </c>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
@@ -4986,7 +5195,9 @@
       <c r="K43" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="L43" s="6"/>
+      <c r="L43" s="9">
+        <v>2</v>
+      </c>
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
@@ -5039,7 +5250,9 @@
       <c r="K44" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="L44" s="6"/>
+      <c r="L44" s="9">
+        <v>2</v>
+      </c>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
@@ -5092,7 +5305,9 @@
       <c r="K45" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="L45" s="26"/>
+      <c r="L45" s="9">
+        <v>2</v>
+      </c>
       <c r="M45" s="26"/>
       <c r="N45" s="26"/>
       <c r="O45" s="26"/>
@@ -5145,7 +5360,9 @@
       <c r="K46" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="L46" s="6"/>
+      <c r="L46" s="9">
+        <v>2</v>
+      </c>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
@@ -5198,7 +5415,9 @@
       <c r="K47" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L47" s="26"/>
+      <c r="L47" s="9">
+        <v>2</v>
+      </c>
       <c r="M47" s="26"/>
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
@@ -5251,7 +5470,9 @@
       <c r="K48" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="L48" s="26"/>
+      <c r="L48" s="9">
+        <v>2</v>
+      </c>
       <c r="M48" s="26"/>
       <c r="N48" s="26"/>
       <c r="O48" s="26"/>
@@ -5270,7 +5491,7 @@
       <c r="AB48" s="26"/>
       <c r="AC48" s="26"/>
     </row>
-    <row r="49" spans="1:29" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" ht="255" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>226</v>
       </c>
@@ -5304,7 +5525,9 @@
       <c r="K49" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="L49" s="6"/>
+      <c r="L49" s="9">
+        <v>2</v>
+      </c>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
@@ -5357,7 +5580,9 @@
       <c r="K50" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L50" s="6"/>
+      <c r="L50" s="9">
+        <v>2</v>
+      </c>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
@@ -5410,7 +5635,9 @@
       <c r="K51" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="L51" s="26"/>
+      <c r="L51" s="9">
+        <v>2</v>
+      </c>
       <c r="M51" s="26"/>
       <c r="N51" s="26"/>
       <c r="O51" s="26"/>
@@ -5429,7 +5656,7 @@
       <c r="AB51" s="26"/>
       <c r="AC51" s="26"/>
     </row>
-    <row r="52" spans="1:29" ht="408" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
         <v>235</v>
       </c>
@@ -5463,7 +5690,9 @@
       <c r="K52" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="L52" s="26"/>
+      <c r="L52" s="9">
+        <v>2</v>
+      </c>
       <c r="M52" s="26"/>
       <c r="N52" s="26"/>
       <c r="O52" s="26"/>
@@ -5482,7 +5711,7 @@
       <c r="AB52" s="26"/>
       <c r="AC52" s="26"/>
     </row>
-    <row r="53" spans="1:29" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>238</v>
       </c>
@@ -5516,7 +5745,9 @@
       <c r="K53" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L53" s="6"/>
+      <c r="L53" s="9">
+        <v>2</v>
+      </c>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
@@ -5535,7 +5766,7 @@
       <c r="AB53" s="6"/>
       <c r="AC53" s="6"/>
     </row>
-    <row r="54" spans="1:29" ht="255" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" ht="267.75" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>243</v>
       </c>
@@ -5569,7 +5800,9 @@
       <c r="K54" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L54" s="6"/>
+      <c r="L54" s="9">
+        <v>2</v>
+      </c>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
@@ -5622,7 +5855,9 @@
       <c r="K55" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L55" s="6"/>
+      <c r="L55" s="9">
+        <v>2</v>
+      </c>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
@@ -5641,7 +5876,7 @@
       <c r="AB55" s="6"/>
       <c r="AC55" s="6"/>
     </row>
-    <row r="56" spans="1:29" ht="395.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>249</v>
       </c>
@@ -5675,7 +5910,9 @@
       <c r="K56" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="L56" s="6"/>
+      <c r="L56" s="9">
+        <v>2</v>
+      </c>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
@@ -5694,7 +5931,7 @@
       <c r="AB56" s="6"/>
       <c r="AC56" s="6"/>
     </row>
-    <row r="57" spans="1:29" ht="395.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>255</v>
       </c>
@@ -5728,7 +5965,9 @@
       <c r="K57" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L57" s="28"/>
+      <c r="L57" s="9">
+        <v>2</v>
+      </c>
       <c r="M57" s="28"/>
       <c r="N57" s="28"/>
       <c r="O57" s="28"/>
@@ -5747,7 +5986,7 @@
       <c r="AB57" s="28"/>
       <c r="AC57" s="28"/>
     </row>
-    <row r="58" spans="1:29" ht="408" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>258</v>
       </c>
@@ -5781,7 +6020,9 @@
       <c r="K58" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L58" s="8"/>
+      <c r="L58" s="9">
+        <v>2</v>
+      </c>
       <c r="M58" s="8"/>
       <c r="N58" s="8"/>
       <c r="O58" s="10"/>
@@ -5834,7 +6075,9 @@
       <c r="K59" s="25" t="s">
         <v>267</v>
       </c>
-      <c r="L59" s="26"/>
+      <c r="L59" s="9">
+        <v>2</v>
+      </c>
       <c r="M59" s="26"/>
       <c r="N59" s="26"/>
       <c r="O59" s="26"/>
@@ -5887,7 +6130,9 @@
       <c r="K60" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="L60" s="6"/>
+      <c r="L60" s="9">
+        <v>2</v>
+      </c>
       <c r="M60" s="6"/>
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
@@ -5940,7 +6185,9 @@
       <c r="K61" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="L61" s="6"/>
+      <c r="L61" s="9">
+        <v>2</v>
+      </c>
       <c r="M61" s="6"/>
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>
@@ -5959,7 +6206,7 @@
       <c r="AB61" s="6"/>
       <c r="AC61" s="6"/>
     </row>
-    <row r="62" spans="1:29" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
         <v>276</v>
       </c>
@@ -5993,7 +6240,9 @@
       <c r="K62" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L62" s="6"/>
+      <c r="L62" s="9">
+        <v>2</v>
+      </c>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
@@ -6012,7 +6261,7 @@
       <c r="AB62" s="6"/>
       <c r="AC62" s="6"/>
     </row>
-    <row r="63" spans="1:29" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>279</v>
       </c>
@@ -6046,7 +6295,9 @@
       <c r="K63" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="L63" s="6"/>
+      <c r="L63" s="9">
+        <v>2</v>
+      </c>
       <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
@@ -6099,7 +6350,9 @@
       <c r="K64" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="L64" s="6"/>
+      <c r="L64" s="9">
+        <v>2</v>
+      </c>
       <c r="M64" s="6"/>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
@@ -6152,7 +6405,9 @@
       <c r="K65" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="L65" s="6"/>
+      <c r="L65" s="9">
+        <v>2</v>
+      </c>
       <c r="M65" s="6"/>
       <c r="N65" s="6"/>
       <c r="O65" s="6"/>
@@ -6205,7 +6460,9 @@
       <c r="K66" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="L66" s="6"/>
+      <c r="L66" s="9">
+        <v>2</v>
+      </c>
       <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
@@ -6224,7 +6481,7 @@
       <c r="AB66" s="6"/>
       <c r="AC66" s="6"/>
     </row>
-    <row r="67" spans="1:29" ht="344.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" ht="357" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>298</v>
       </c>
@@ -6258,7 +6515,9 @@
       <c r="K67" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L67" s="6"/>
+      <c r="L67" s="9">
+        <v>2</v>
+      </c>
       <c r="M67" s="6"/>
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
@@ -6311,7 +6570,9 @@
       <c r="K68" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="L68" s="6"/>
+      <c r="L68" s="9">
+        <v>2</v>
+      </c>
       <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
@@ -6364,7 +6625,9 @@
       <c r="K69" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="L69" s="6"/>
+      <c r="L69" s="9">
+        <v>2</v>
+      </c>
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
@@ -6417,7 +6680,9 @@
       <c r="K70" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="L70" s="6"/>
+      <c r="L70" s="9">
+        <v>2</v>
+      </c>
       <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
@@ -6436,7 +6701,7 @@
       <c r="AB70" s="6"/>
       <c r="AC70" s="6"/>
     </row>
-    <row r="71" spans="1:29" ht="280.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" ht="293.25" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>318</v>
       </c>
@@ -6470,7 +6735,9 @@
       <c r="K71" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="L71" s="6"/>
+      <c r="L71" s="9">
+        <v>2</v>
+      </c>
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
@@ -6523,7 +6790,9 @@
       <c r="K72" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="L72" s="6"/>
+      <c r="L72" s="9">
+        <v>2</v>
+      </c>
       <c r="M72" s="6"/>
       <c r="N72" s="6"/>
       <c r="O72" s="6"/>
@@ -36181,7 +36450,7 @@
   </sheetData>
   <autoFilter ref="A1:G72"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>